<commit_message>
Deadlines over a day include hours
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -37,31 +37,131 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>say hi</t>
-  </si>
-  <si>
-    <t>due today</t>
-  </si>
-  <si>
-    <t>a greeting</t>
+    <t>Virtual Desk Timeout</t>
+  </si>
+  <si>
+    <t>Data Transfer Rate</t>
+  </si>
+  <si>
+    <t>Better QC Tool</t>
+  </si>
+  <si>
+    <t>Automate Signout Checklist</t>
+  </si>
+  <si>
+    <t>Increase CPU Power</t>
+  </si>
+  <si>
+    <t>ngjob file sample order</t>
+  </si>
+  <si>
+    <t>Primer Seek</t>
+  </si>
+  <si>
+    <t>Automate Execution of NextGene</t>
+  </si>
+  <si>
+    <t>BAMasker/BRR One-click</t>
+  </si>
+  <si>
+    <t>Automate data transfer</t>
+  </si>
+  <si>
+    <t>Automate VCF Upload Annotation</t>
+  </si>
+  <si>
+    <t>NonCode</t>
+  </si>
+  <si>
+    <t>NoneCode</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>2018-08-09
+10:00
+2 days left!</t>
   </si>
   <si>
     <t>2018-08-10
-11:00
+12:00
 3 days left!</t>
   </si>
   <si>
-    <t>2018-08-07
+    <t>2018-08-11
+14:00
+5 days and 0 hours left!</t>
+  </si>
+  <si>
+    <t>2018-08-12
+08:00
+5 days and 18 hours left!</t>
+  </si>
+  <si>
+    <t>2018-08-13
+23:00
+7 days and 9 hours left!</t>
+  </si>
+  <si>
+    <t>2018-08-15
+03:00
+8 days and 13 hours left!</t>
+  </si>
+  <si>
+    <t>2018-08-20
+12:00
+13 days and 22 hours left!</t>
+  </si>
+  <si>
+    <t>2018-08-01
 10:00
-22 hours left!</t>
+Task is past due</t>
+  </si>
+  <si>
+    <t>2018-08-05
+00:00
+Task is past due</t>
   </si>
   <si>
     <t>2018-08-06
-14:00
+10:00
+Task is past due</t>
+  </si>
+  <si>
+    <t>2018-08-06
+17:00
 Due today!</t>
+  </si>
+  <si>
+    <t>work/misc</t>
   </si>
   <si>
     <t>None</t>
@@ -422,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,22 +559,22 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -485,22 +585,22 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -511,22 +611,230 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>